<commit_message>
Re-publish with updated extensions
</commit_message>
<xml_diff>
--- a/docs/Extension-UKCore-ListWarningCode.xlsx
+++ b/docs/Extension-UKCore-ListWarningCode.xlsx
@@ -134,16 +134,13 @@
     <t>0</t>
   </si>
   <si>
-    <t>1</t>
+    <t>*</t>
   </si>
   <si>
     <t>To capture warnings that the list may be incomplete</t>
   </si>
   <si>
     <t>To capture warnings that the list may be incomplete.</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Extension.id</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t xml:space="preserve">string
@@ -639,13 +639,13 @@
         <v>38</v>
       </c>
       <c r="AG2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH2" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="AH2" t="s" s="2">
+      <c r="AI2" t="s" s="2">
         <v>43</v>
-      </c>
-      <c r="AI2" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="AJ2" t="s" s="2">
         <v>37</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -664,7 +664,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>37</v>
@@ -739,7 +739,7 @@
         <v>38</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>37</v>
@@ -764,7 +764,7 @@
         <v>38</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>37</v>
@@ -841,13 +841,13 @@
         <v>38</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AH4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>50</v>
@@ -863,10 +863,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>37</v>
@@ -940,10 +940,10 @@
         <v>61</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>37</v>
@@ -965,10 +965,10 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>37</v>
@@ -1043,7 +1043,7 @@
         <v>38</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>37</v>

</xml_diff>